<commit_message>
Support ApiError conversion to XLSX
</commit_message>
<xml_diff>
--- a/src/test/resources/ApiError.xlsx
+++ b/src/test/resources/ApiError.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eberleant/Work/Galatea/galatea-associates/fuse-starter-java/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F1BA47D-F56D-C748-A90B-0A95051207A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE931A0B-046C-9D4A-857A-F3CFF348A2B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="920" windowWidth="27640" windowHeight="16540" xr2:uid="{7D69362E-3D77-714B-A840-543A23C503FA}"/>
+    <workbookView xWindow="1160" yWindow="920" windowWidth="27640" windowHeight="16540" xr2:uid="{7D69362E-3D77-714B-A840-543A23C503FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>message</t>
   </si>
   <si>
-    <t>NOT_FOUND</t>
+    <t>org.galatea.starter.entrypoint.exception.EntityNotFoundException: Entities [1, 2] of type SettlementMission were not found</t>
   </si>
   <si>
-    <t>org.galatea.starter.entrypoint.exception.EntityNotFoundException: Entities [1, 2] of type SettlementMission were not found</t>
+    <t>404 NOT_FOUND</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -406,10 +406,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>